<commit_message>
Updated my log and hours.
</commit_message>
<xml_diff>
--- a/Documentation/JulianSkeleWarHours.xlsx
+++ b/Documentation/JulianSkeleWarHours.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>Day</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t>Week 5</t>
+  </si>
+  <si>
+    <t>Week 6</t>
   </si>
 </sst>
 </file>
@@ -404,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -824,25 +827,58 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
+      <c r="A27" s="6" t="s">
+        <v>11</v>
+      </c>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="5"/>
       <c r="E27" s="4"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="4"/>
+      <c r="A28" s="2">
+        <v>42244</v>
+      </c>
+      <c r="B28" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="C28" s="3">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="D28" s="5">
+        <v>0</v>
+      </c>
+      <c r="E28" s="4">
+        <f t="shared" ref="E28:E29" si="3">MOD(C28-B28,1)*24-D28</f>
+        <v>5.0000000000000009</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="4"/>
+      <c r="A29" s="2">
+        <v>42247</v>
+      </c>
+      <c r="B29" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C29" s="3">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="D29" s="5">
+        <v>2</v>
+      </c>
+      <c r="E29" s="4">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D30" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E30" s="8">
+        <f>SUM(E28:E29)</f>
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated my progress log and hours.
</commit_message>
<xml_diff>
--- a/Documentation/JulianSkeleWarHours.xlsx
+++ b/Documentation/JulianSkeleWarHours.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t>Day</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t>Week 6</t>
+  </si>
+  <si>
+    <t>Week 7</t>
   </si>
 </sst>
 </file>
@@ -407,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -880,6 +883,56 @@
         <v>14</v>
       </c>
     </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>42253</v>
+      </c>
+      <c r="B32" s="3">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="C32" s="3">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="D32" s="5">
+        <v>0</v>
+      </c>
+      <c r="E32" s="4">
+        <f>MOD(C32-B32,1)*24-D32</f>
+        <v>4.0000000000000018</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>42254</v>
+      </c>
+      <c r="B33" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="C33" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="D33" s="5">
+        <v>1</v>
+      </c>
+      <c r="E33" s="4">
+        <f>MOD(C33-B33,1)*24-D33</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D34" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E34" s="8">
+        <f>SUM(E32:E33)</f>
+        <v>15.000000000000002</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated my progress log.
</commit_message>
<xml_diff>
--- a/Documentation/JulianSkeleWarHours.xlsx
+++ b/Documentation/JulianSkeleWarHours.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>Day</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t>Week 7</t>
+  </si>
+  <si>
+    <t>Week 8</t>
   </si>
 </sst>
 </file>
@@ -410,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -933,6 +936,74 @@
         <v>15.000000000000002</v>
       </c>
     </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>42258</v>
+      </c>
+      <c r="B36" s="3">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="C36" s="3">
+        <v>0</v>
+      </c>
+      <c r="D36" s="5">
+        <v>0</v>
+      </c>
+      <c r="E36" s="4">
+        <f>MOD(C36-B36,1)*24-D36</f>
+        <v>2.0000000000000009</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>42260</v>
+      </c>
+      <c r="B37" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C37" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D37" s="5">
+        <v>2</v>
+      </c>
+      <c r="E37" s="4">
+        <f>MOD(C37-B37,1)*24-D37</f>
+        <v>11.000000000000002</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>42261</v>
+      </c>
+      <c r="B38" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C38" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D38" s="5">
+        <v>1</v>
+      </c>
+      <c r="E38" s="4">
+        <f t="shared" ref="E38:E39" si="4">MOD(C38-B38,1)*24-D38</f>
+        <v>12.000000000000002</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D39" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E39" s="8">
+        <f>SUM(E36:E38)</f>
+        <v>25.000000000000007</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>